<commit_message>
0.9.8 - complete rewrite
Completely rewritten from scratch. Yeah, go figure.
After reading Hadley Wickham's "Tiday Data" while in the process of
writing a dplyr script to calculate D scores, I realised that the block
layout of the task was a shambles.

With some thought, and the idea that I could use an excel file and loop
to specify which excel file the loop below should pull from, I managed
to reduce the builder flow from many routines to just three. Similarly,
the py script went from 1850 lines to 450, and is also much more
readable.

This is not just code aesthetics however: the data file now has no
empty cells. This is in line with the Tidy Data concept that each
variable should form a single column. For example, previously, a given
RT column contained the reaction times *but also* specified which block
they were from, making it harder to analyse the data. Instead, a second
variable (e.g., blocks.thisRepN) now specifies the block. This makes
analysis easier.
</commit_message>
<xml_diff>
--- a/Dutch translation files/instructions.xlsx
+++ b/Dutch translation files/instructions.xlsx
@@ -19,19 +19,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>instructions</t>
   </si>
   <si>
-    <t xml:space="preserve">Goed gedaan!
-Dit is het einde van deze taak. </t>
+    <t>stimulusFile</t>
+  </si>
+  <si>
+    <t>stimuliBlock1.xlsx</t>
+  </si>
+  <si>
+    <t>stimuliBlock2.xlsx</t>
+  </si>
+  <si>
+    <t>stimuliBlock3.xlsx</t>
+  </si>
+  <si>
+    <t>stimuliBlock4.xlsx</t>
+  </si>
+  <si>
+    <t>stimuliBlock5.xlsx</t>
+  </si>
+  <si>
+    <t>nBlockRepetitions</t>
   </si>
   <si>
     <t xml:space="preserve">In dit reactietijdexperiment zal U moeten reageren op woorden en stellingen die aangeboden worden op het scherm. In de eerstvolgende fase zullen woorden aangeboden worden in het ORANJE.
 Het is uw taak om zo snel mogelijk te bepalen of het woord verwijst naar WAAR of naar NIET WAAR.
 Druk op de I-toets als de woord een synoniem van WAAR is.
 Druk op de E-toets als de woord een synoniem van NIET WAAR is.
+Mocht U een fout maken druk dan alsnog zo snel mogelijk de juiste toets in!
+Zet uw beide wijsvingers op de E en I toetsen. Druk op de ene naar de volgende fase te starten. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In de volgende fase zullen stellingen aangeboden worden. Deze stellingen zullen in het BLAUW gepresenteerd worden en zijn altijd stellingen over zelfwaarde.
+Wanneer U een stelling in het blauw ziet dient U te reageren ALSOF 'Ik ben en wil goed zijn en niet slecht'.
+Druk op de rechter I-toets wanneer de stelling WAAR is op basis van bovengenoemde regel.
+Druk op de linker E-toets wanneer de stelling NIET WAAR is op basis van bovengenoemde regel. 
+Bijvoorbeeld:
+Wanneer U de stelling 'Ik ben waardevol' te zien zou krijgen reageer dan met de respons 'WAAR' (rechter I-toets). 
+Wanneer U de stelling 'Ik ben mislukt' te zien zou krijgen reageer dan met de respons 'NIET WAAR' (linker E-toets).
 Mocht U een fout maken druk dan alsnog zo snel mogelijk de juiste toets in!
 Zet uw beide wijsvingers op de E en I toetsen. Druk op de ene naar de volgende fase te starten. </t>
   </si>
@@ -67,17 +95,6 @@
 Druk op de linker E-toets als de woord een synoniem van NIET WAAR is.
 Mocht U een fout maken druk dan alsnog zo snel mogelijk de juiste toets in!
 Zet uw beide wijsvingers op de E en I toetsen. Druk op de ene naar de volgende fase te starten.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In de volgende fase zullen stellingen aangeboden worden. Deze stellingen zullen in het BLAUW gepresenteerd worden en zijn altijd stellingen over zelfwaarde.
-Wanneer U een stelling in het blauw ziet dient U te reageren ALSOF 'Ik ben en wil goed zijn en niet slecht'.
-Druk op de rechter I-toets wanneer de stelling WAAR is op basis van bovengenoemde regel.
-Druk op de linker E-toets wanneer de stelling NIET WAAR is op basis van bovengenoemde regel. 
-Bijvoorbeeld:
-Wanneer U de stelling 'Ik ben waardevol' te zien zou krijgen reageer dan met de respons 'WAAR' (rechter I-toets). 
-Wanneer U de stelling 'Ik ben mislukt' te zien zou krijgen reageer dan met de respons 'NIET WAAR' (linker E-toets).
-Mocht U een fout maken druk dan alsnog zo snel mogelijk de juiste toets in!
-Zet uw beide wijsvingers op de E en I toetsen. Druk op de ene naar de volgende fase te starten. </t>
   </si>
 </sst>
 </file>
@@ -135,7 +152,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="137">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -237,53 +254,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -292,7 +267,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="137">
+  <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -343,24 +318,6 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -411,24 +368,6 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -761,53 +700,83 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="64.1640625" customWidth="1"/>
-    <col min="2" max="2" width="61.5" customWidth="1"/>
-    <col min="3" max="3" width="72.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="79.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="210">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" ht="195">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="C2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="330">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" ht="270">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="255">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="255">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="255">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4"/>
+      <c r="C6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="300">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="300">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="300">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>